<commit_message>
Import harvester details and replace the tractor data.
</commit_message>
<xml_diff>
--- a/Content/Harvester/Harvester_Infos1.xlsx
+++ b/Content/Harvester/Harvester_Infos1.xlsx
@@ -14,27 +14,84 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="140">
   <si>
     <t>Kartar</t>
   </si>
   <si>
+    <t>Vishal</t>
+  </si>
+  <si>
+    <t>Preet</t>
+  </si>
+  <si>
+    <t>Mahindra</t>
+  </si>
+  <si>
+    <t>Kubota</t>
+  </si>
+  <si>
     <t>4000</t>
   </si>
   <si>
+    <t>435</t>
+  </si>
+  <si>
+    <t>987</t>
+  </si>
+  <si>
+    <t>MSI 457 3A</t>
+  </si>
+  <si>
+    <t>HARVESKING DC-68G-HK</t>
+  </si>
+  <si>
     <t>['img0-40009999.png']</t>
   </si>
   <si>
+    <t>['img0-435-1647923189.png']</t>
+  </si>
+  <si>
+    <t>['img0-987-1646896081.png']</t>
+  </si>
+  <si>
+    <t>['img0-arjun-6059999.png']</t>
+  </si>
+  <si>
+    <t>['img0-harvesking-dc-68g-hk-1647922688.png']</t>
+  </si>
+  <si>
     <t>14 Feet</t>
   </si>
   <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>14 feet(4.3 m)</t>
+  </si>
+  <si>
+    <t>11.81 Feet</t>
+  </si>
+  <si>
+    <t>900 x 1903 MM</t>
+  </si>
+  <si>
     <t>6</t>
   </si>
   <si>
     <t>Self Propelled</t>
   </si>
   <si>
+    <t>Tractor Mounted</t>
+  </si>
+  <si>
     <t>Multicrop</t>
+  </si>
+  <si>
+    <t>MultiCrop</t>
+  </si>
+  <si>
+    <t>Paddy</t>
   </si>
   <si>
     <t>Kartar 4000 Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Kartar 4000 Multicrop harvester for their farms. In addition, Kartar 4000 harvester features are also excellent. That’s why the Kartar 4000 harvester machine is one of India's most preferred farming machines. Kartar 4000 price 2024 is also valuable for farmers. Moreover, the Kartar 4000 harvester machine is filled with highly modern technology to serve better in the field.
@@ -46,69 +103,252 @@
 You can get a reliable Kartar 4000 combine price at Tractor Junction. Here we are with complete details of this harvester, including Kartar 4000 combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Kartar 4000 combine on road price at your place.</t>
   </si>
   <si>
+    <t>Vishal 435 Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Vishal 435 MultiCrop harvester for their farms. In addition, Vishal 435 harvester features are also excellent. That’s why the Vishal 435 harvester machine is one of India's most preferred farming machines. Vishal 435 price 2024 is also valuable for farmers. Moreover, the Vishal 435 harvester machine is filled with highly modern technology to serve better in the field.
+Vishal 435 MultiCrop Combine Harvester Price
+Vishal 435 MultiCrop combine harvester price is valuable to the Indian farmers. You can also get a complete Vishal 435 combine harvester price list at Tractor Junction. On the other hand, the Vishal 435 combine on road price can differ from state to state due to several factors.
+Vishal 435 Harvester Features
+Let’s know the Vishal 435 harvester features. The working efficiency and performance of Vishal 435 Tractor Harvester are also excellent. The engine of this Vishal 435 has enormous power and comes at value for money Vishal 435 combine price. So, let’s know more about Vishal 435 MultiCrop harvester at Tractor Junction.
+Vishal 435 Combine Harvester Price at Tractor Junction
+You can get a reliable Vishal 435 combine price at Tractor Junction. Here we are with complete details of this harvester, including Vishal 435 combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Vishal 435 combine on road price at your place.</t>
+  </si>
+  <si>
+    <t>Preet 987 Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Preet 987 Multicrop harvester for their farms. In addition, Preet 987 harvester features are also excellent. That’s why the Preet 987 harvester machine is one of India's most preferred farming machines. Preet 987 price 2024 is also valuable for farmers. Moreover, the Preet 987 harvester machine is filled with highly modern technology to serve better in the field.
+Preet 987 Multicrop Combine Harvester Price
+Preet 987 Multicrop combine harvester price is valuable to the Indian farmers. You can also get a complete Preet 987 combine harvester price list at Tractor Junction. On the other hand, the Preet 987 combine on road price can differ from state to state due to several factors.
+Preet 987 Harvester Features
+Let’s know the Preet 987 harvester features. The working efficiency and performance of Preet 987 Tractor Harvester are also excellent. The engine of this Preet 987 has enormous power and comes at value for money Preet 987 combine price. So, let’s know more about Preet 987 Multicrop harvester at Tractor Junction.
+Preet 987 Combine Harvester Price at Tractor Junction
+You can get a reliable Preet 987 combine price at Tractor Junction. Here we are with complete details of this harvester, including Preet 987 combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Preet 987 combine on road price at your place.</t>
+  </si>
+  <si>
+    <t>Mahindra MSI 457 3A Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Mahindra MSI 457 3A Multicrop harvester for their farms. In addition, Mahindra MSI 457 3A harvester features are also excellent. That’s why the Mahindra MSI 457 3A harvester machine is one of India's most preferred farming machines. Mahindra MSI 457 3A price 2024 is also valuable for farmers. Moreover, the Mahindra MSI 457 3A harvester machine is filled with highly modern technology to serve better in the field.
+Mahindra MSI 457 3A Multicrop Combine Harvester Price
+Mahindra MSI 457 3A Multicrop combine harvester price is valuable to the Indian farmers. You can also get a complete Mahindra MSI 457 3A combine harvester price list at Tractor Junction. On the other hand, the Mahindra MSI 457 3A combine on road price can differ from state to state due to several factors.
+Mahindra MSI 457 3A Harvester Features
+Let’s know the Mahindra MSI 457 3A harvester features. The working efficiency and performance of Mahindra MSI 457 3A Tractor Harvester are also excellent. The engine of this Mahindra MSI 457 3A has enormous power and comes at value for money Mahindra MSI 457 3A combine price. So, let’s know more about Mahindra MSI 457 3A Multicrop harvester at Tractor Junction.
+Mahindra MSI 457 3A Combine Harvester Price at Tractor Junction
+You can get a reliable Mahindra MSI 457 3A combine price at Tractor Junction. Here we are with complete details of this harvester, including Mahindra MSI 457 3A combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Mahindra MSI 457 3A combine on road price at your place.</t>
+  </si>
+  <si>
+    <t>Kubota HARVESKING DC-68G-HK Tractor Harvester is an efficient machine for farming in India. The farmers are extensively using Kubota HARVESKING DC-68G-HK Paddy harvester for their farms. In addition, Kubota HARVESKING DC-68G-HK harvester features are also excellent. That’s why the Kubota HARVESKING DC-68G-HK harvester machine is one of India's most preferred farming machines. Kubota HARVESKING DC-68G-HK price 2024 is also valuable for farmers. Moreover, the Kubota HARVESKING DC-68G-HK harvester machine is filled with highly modern technology to serve better in the field.
+Kubota HARVESKING DC-68G-HK Paddy Combine Harvester Price
+Kubota HARVESKING DC-68G-HK Paddy combine harvester price is valuable to the Indian farmers. You can also get a complete Kubota HARVESKING DC-68G-HK combine harvester price list at Tractor Junction. On the other hand, the Kubota HARVESKING DC-68G-HK combine on road price can differ from state to state due to several factors.
+Kubota HARVESKING DC-68G-HK Harvester Features
+Let’s know the Kubota HARVESKING DC-68G-HK harvester features. The working efficiency and performance of Kubota HARVESKING DC-68G-HK Tractor Harvester are also excellent. The engine of this Kubota HARVESKING DC-68G-HK has enormous power and comes at value for money Kubota HARVESKING DC-68G-HK combine price. So, let’s know more about Kubota HARVESKING DC-68G-HK Paddy harvester at Tractor Junction.
+Kubota HARVESKING DC-68G-HK Combine Harvester Price at Tractor Junction
+You can get a reliable Kubota HARVESKING DC-68G-HK combine price at Tractor Junction. Here we are with complete details of this harvester, including Kubota HARVESKING DC-68G-HK combine price 2024, specifications and others. Apart from this, you can also call us to get genuine Kubota HARVESKING DC-68G-HK combine on road price at your place.</t>
+  </si>
+  <si>
     <t>Ashok Leyland
 H6ET1C3RD22/1
 101 H.P @2200
 RPM</t>
   </si>
   <si>
+    <t xml:space="preserve">Ashok Leyland </t>
+  </si>
+  <si>
+    <t>Water-Cooled 4-Cycle 4-Cylinder Vertical Diesel Engine[WithTurbocharger]</t>
+  </si>
+  <si>
     <t>101 HP</t>
   </si>
   <si>
+    <t>101</t>
+  </si>
+  <si>
+    <t>68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.9 Ltr. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combination of Dry &amp; Wet Type </t>
+  </si>
+  <si>
     <t>100 mm</t>
   </si>
   <si>
+    <t>65-1275</t>
+  </si>
+  <si>
+    <t>-819</t>
+  </si>
+  <si>
     <t>700 mm</t>
   </si>
   <si>
     <t>Hydraulically</t>
   </si>
   <si>
+    <t>Hydraulics</t>
+  </si>
+  <si>
     <t>Pick Up</t>
   </si>
   <si>
     <t>Mechanically</t>
   </si>
   <si>
+    <t xml:space="preserve">By means of Mechanical Variator </t>
+  </si>
+  <si>
     <t>Water Cooled</t>
   </si>
   <si>
+    <t xml:space="preserve">Water Cooled </t>
+  </si>
+  <si>
+    <t>14 Feet (4.3m)</t>
+  </si>
+  <si>
+    <t>1250</t>
+  </si>
+  <si>
+    <t>234</t>
+  </si>
+  <si>
+    <t>4665</t>
+  </si>
+  <si>
+    <t>2,245</t>
+  </si>
+  <si>
+    <t>1375 x 840</t>
+  </si>
+  <si>
     <t>1270 mm</t>
   </si>
   <si>
     <t>600 mm</t>
   </si>
   <si>
+    <t xml:space="preserve">Mechanical </t>
+  </si>
+  <si>
     <t>16 to 39 mm</t>
   </si>
   <si>
     <t>2.64 meter Cube</t>
   </si>
   <si>
+    <t>2.180 m2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.5 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Forward + 1 Reverse </t>
+  </si>
+  <si>
+    <t>Traveling Speed (m/s) F/R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Single, Heavy Duty Dry Clutch </t>
+  </si>
+  <si>
     <t>18.4/15/30</t>
   </si>
   <si>
+    <t>18.4 / 15 / 30</t>
+  </si>
+  <si>
+    <t>18.4 / 15 x 30</t>
+  </si>
+  <si>
     <t>9.00 X 16</t>
   </si>
   <si>
+    <t>7 x 50 x 16</t>
+  </si>
+  <si>
+    <t>9.00 x 16</t>
+  </si>
+  <si>
     <t>380 Lts.</t>
   </si>
   <si>
+    <t>365</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
     <t>9150 Kgs. (Approx.)</t>
   </si>
   <si>
+    <t>8500</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
     <t>8535 mm</t>
   </si>
   <si>
+    <t>8340 mm</t>
+  </si>
+  <si>
     <t>4572 mm</t>
   </si>
   <si>
+    <t>3787 mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3800 </t>
+  </si>
+  <si>
+    <t>3710mm</t>
+  </si>
+  <si>
+    <t>2,800</t>
+  </si>
+  <si>
     <t>4199 mm</t>
   </si>
   <si>
+    <t>4665 mm</t>
+  </si>
+  <si>
+    <t>11.25 Feet (3.4m), 10.25 Feet (3.12m)</t>
+  </si>
+  <si>
+    <t>2565mm</t>
+  </si>
+  <si>
     <t>460 mm</t>
   </si>
   <si>
+    <t>370 mm</t>
+  </si>
+  <si>
+    <t>340</t>
+  </si>
+  <si>
+    <t>325</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
     <t>Brand</t>
   </si>
   <si>
@@ -163,6 +403,15 @@
     <t>Reel_Speed_Adjustment</t>
   </si>
   <si>
+    <t>Max_Revolution</t>
+  </si>
+  <si>
+    <t>Min_Revolution</t>
+  </si>
+  <si>
+    <t>Reel_Height_Adjustment</t>
+  </si>
+  <si>
     <t>Cooling_System</t>
   </si>
   <si>
@@ -215,6 +464,9 @@
   </si>
   <si>
     <t>Ground_Clearance</t>
+  </si>
+  <si>
+    <t>Image_Type_Nmae</t>
   </si>
 </sst>
 </file>
@@ -570,209 +822,504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AN10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:40">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>101</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>30</v>
+        <v>102</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>31</v>
+        <v>103</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>38</v>
+        <v>110</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>39</v>
+        <v>111</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>40</v>
+        <v>112</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>43</v>
+        <v>115</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>44</v>
+        <v>116</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>46</v>
+        <v>118</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>47</v>
+        <v>119</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>48</v>
+        <v>120</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>49</v>
+        <v>121</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>50</v>
+        <v>122</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>51</v>
+        <v>123</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>52</v>
+        <v>124</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>53</v>
+        <v>125</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>54</v>
+        <v>126</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>56</v>
+        <v>128</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>57</v>
+        <v>129</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>58</v>
+        <v>130</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>59</v>
+        <v>131</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>60</v>
+        <v>132</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>61</v>
+        <v>133</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>63</v>
+        <v>135</v>
+      </c>
+      <c r="AK1" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AM1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AN1" s="1" t="s">
+        <v>139</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:40">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>39</v>
+      </c>
+      <c r="N2" t="s">
+        <v>42</v>
+      </c>
+      <c r="O2" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" t="s">
+        <v>45</v>
+      </c>
+      <c r="R2" t="s">
+        <v>46</v>
+      </c>
+      <c r="V2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>46</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:40">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="V3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>67</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>70</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>76</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>79</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>86</v>
+      </c>
+      <c r="AM3" t="s">
+        <v>90</v>
+      </c>
+      <c r="AN3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:40">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H4" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" t="s">
+        <v>35</v>
+      </c>
+      <c r="L4" t="s">
+        <v>38</v>
+      </c>
+      <c r="M4" t="s">
+        <v>40</v>
+      </c>
+      <c r="R4" t="s">
+        <v>47</v>
+      </c>
+      <c r="V4" t="s">
+        <v>49</v>
+      </c>
+      <c r="X4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>71</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>77</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>82</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>50</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AN4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:40">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="E2" t="s">
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s">
+        <v>16</v>
+      </c>
+      <c r="X5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>63</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>83</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>87</v>
+      </c>
+      <c r="AN5" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:40">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="M2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P2" t="s">
-        <v>13</v>
-      </c>
-      <c r="R2" t="s">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="S2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="D6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" t="s">
         <v>16</v>
       </c>
-      <c r="W2" t="s">
-        <v>17</v>
-      </c>
-      <c r="X2" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>18</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>19</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD2" t="s">
+      <c r="F6" t="s">
         <v>21</v>
       </c>
-      <c r="AE2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>23</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AH2" t="s">
+      <c r="G6" t="s">
         <v>25</v>
       </c>
-      <c r="AI2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>27</v>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" t="s">
+        <v>36</v>
+      </c>
+      <c r="M6" t="s">
+        <v>41</v>
+      </c>
+      <c r="O6" t="s">
+        <v>44</v>
+      </c>
+      <c r="X6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>84</v>
+      </c>
+      <c r="AL6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM6" t="s">
+        <v>92</v>
+      </c>
+      <c r="AN6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:40">
+      <c r="X7" t="s">
+        <v>53</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>52</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40">
+      <c r="AL8" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:40">
+      <c r="X9" t="s">
+        <v>54</v>
+      </c>
+      <c r="AL9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40">
+      <c r="X10" t="s">
+        <v>55</v>
+      </c>
+      <c r="AL10" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>